<commit_message>
added first series of MC3PO targets to reduction_status_list
</commit_message>
<xml_diff>
--- a/Reduction Notes/Reduction_Status_List.xlsx
+++ b/Reduction Notes/Reduction_Status_List.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26018"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawson/Git/SuprimeCam/Reduction Notes/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="17420" windowHeight="16880" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="26060" yWindow="8680" windowWidth="17420" windowHeight="16880" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Radio Relic Sample" sheetId="1" r:id="rId1"/>
     <sheet name="MC3PO Sample" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="106">
   <si>
     <t>Semester</t>
   </si>
@@ -199,6 +194,150 @@
   </si>
   <si>
     <t>FRAMID_end</t>
+  </si>
+  <si>
+    <t>SUPA00232340</t>
+  </si>
+  <si>
+    <t>SUPA00232429</t>
+  </si>
+  <si>
+    <t>SUPA00330440</t>
+  </si>
+  <si>
+    <t>SUPA00330529</t>
+  </si>
+  <si>
+    <t>Exposure (s)</t>
+  </si>
+  <si>
+    <t>SUPA00487380</t>
+  </si>
+  <si>
+    <t>SUPA00487459</t>
+  </si>
+  <si>
+    <t>SUPA00557410</t>
+  </si>
+  <si>
+    <t>SUPA00557509</t>
+  </si>
+  <si>
+    <t>SUPA00561680</t>
+  </si>
+  <si>
+    <t>SUPA00561689</t>
+  </si>
+  <si>
+    <t>SUPA00561700</t>
+  </si>
+  <si>
+    <t>SUPA00561709</t>
+  </si>
+  <si>
+    <t>SUPA00561720</t>
+  </si>
+  <si>
+    <t>SUPA00561729</t>
+  </si>
+  <si>
+    <t>SUPA00561740</t>
+  </si>
+  <si>
+    <t>SUPA00561749</t>
+  </si>
+  <si>
+    <t>SUPA00562030</t>
+  </si>
+  <si>
+    <t>SUPA00562109</t>
+  </si>
+  <si>
+    <t>RXC J2228.6+2037</t>
+  </si>
+  <si>
+    <t>RXC J2228.6+2038</t>
+  </si>
+  <si>
+    <t>RXC J2228.6+2039</t>
+  </si>
+  <si>
+    <t>RXC J2228.6+2040</t>
+  </si>
+  <si>
+    <t>RXC J2228.6+2041</t>
+  </si>
+  <si>
+    <t>RXC J2228.6+2042</t>
+  </si>
+  <si>
+    <t>RXC J2228.6+2043</t>
+  </si>
+  <si>
+    <t>RXC J2228.6+2044</t>
+  </si>
+  <si>
+    <t>SUPA00395940</t>
+  </si>
+  <si>
+    <t>SUPA00396029</t>
+  </si>
+  <si>
+    <t>SUPA00022752</t>
+  </si>
+  <si>
+    <t>SUPA00022809</t>
+  </si>
+  <si>
+    <t>SUPA00022852</t>
+  </si>
+  <si>
+    <t>SUPA00022909</t>
+  </si>
+  <si>
+    <t>SUPA00232540</t>
+  </si>
+  <si>
+    <t>SUPA00232559</t>
+  </si>
+  <si>
+    <t>SUPA00242810</t>
+  </si>
+  <si>
+    <t>SUPA00242869</t>
+  </si>
+  <si>
+    <t>SUPA00543720</t>
+  </si>
+  <si>
+    <t>Exposures</t>
+  </si>
+  <si>
+    <t>SUPA00543769</t>
+  </si>
+  <si>
+    <t>SUPA00557520</t>
+  </si>
+  <si>
+    <t>SUPA00557609</t>
+  </si>
+  <si>
+    <t>MACS J2243.3-0936</t>
+  </si>
+  <si>
+    <t>MACS J2243.3-0937</t>
+  </si>
+  <si>
+    <t>MACS J2243.3-0938</t>
+  </si>
+  <si>
+    <t>MACS J2243.3-0939</t>
+  </si>
+  <si>
+    <t>MACS J2243.3-0940</t>
+  </si>
+  <si>
+    <t>Total Exp (m)</t>
   </si>
 </sst>
 </file>
@@ -206,9 +345,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="yyyy\-mmm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mmm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -226,6 +365,22 @@
       <sz val="13"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -245,17 +400,57 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="21">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -311,7 +506,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -346,7 +541,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -523,7 +718,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,7 +732,7 @@
       <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
@@ -549,7 +744,7 @@
     <col min="10" max="10" width="75.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +776,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -605,7 +800,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -629,7 +824,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -653,7 +848,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -675,7 +870,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -695,7 +890,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -715,7 +910,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -739,7 +934,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -765,7 +960,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -789,7 +984,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -813,7 +1008,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -837,7 +1032,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -861,7 +1056,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -885,7 +1080,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -909,7 +1104,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -929,7 +1124,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="3">
         <v>39513</v>
       </c>
@@ -949,7 +1144,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="3">
         <v>40279</v>
       </c>
@@ -969,7 +1164,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="3">
         <v>40637</v>
       </c>
@@ -989,7 +1184,7 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -1013,7 +1208,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -1037,7 +1232,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -1061,7 +1256,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
@@ -1087,7 +1282,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -1109,7 +1304,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -1129,7 +1324,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="2" t="s">
         <v>8</v>
       </c>
@@ -1153,7 +1348,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -1177,7 +1372,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -1199,7 +1394,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -1219,7 +1414,7 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -1243,7 +1438,7 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -1267,7 +1462,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -1291,7 +1486,7 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -1311,7 +1506,7 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
@@ -1331,7 +1526,7 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -1351,7 +1546,7 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -1371,7 +1566,7 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -1393,7 +1588,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="2" t="s">
         <v>34</v>
       </c>
@@ -1413,7 +1608,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="2" t="s">
         <v>34</v>
       </c>
@@ -1433,7 +1628,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="2" t="s">
         <v>34</v>
       </c>
@@ -1453,7 +1648,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="2" t="s">
         <v>34</v>
       </c>
@@ -1475,7 +1670,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="2" t="s">
         <v>34</v>
       </c>
@@ -1495,7 +1690,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="2" t="s">
         <v>34</v>
       </c>
@@ -1517,7 +1712,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="2" t="s">
         <v>34</v>
       </c>
@@ -1537,7 +1732,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="2" t="s">
         <v>34</v>
       </c>
@@ -1559,7 +1754,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="2" t="s">
         <v>34</v>
       </c>
@@ -1579,7 +1774,7 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
         <v>39</v>
@@ -1601,26 +1796,34 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L59"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.1640625" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1640,25 +1843,34 @@
         <v>57</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="A2" s="4">
         <v>38476</v>
       </c>
@@ -1671,11 +1883,28 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2">
+        <f>(RIGHT(F2,LEN(F2)-4)-RIGHT(E2,LEN(E2)-4)+1)/10</f>
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>60</v>
+      </c>
+      <c r="I2">
+        <f>G2*H2/60</f>
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15">
       <c r="A3" s="4">
         <v>37829</v>
       </c>
@@ -1688,247 +1917,601 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G17" si="0">(RIGHT(F3,LEN(F3)-4)-RIGHT(E3,LEN(E3)-4)+1)/10</f>
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>240</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I17" si="1">G3*H3/60</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="4">
         <v>38187</v>
       </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
       <c r="C4" t="s">
         <v>49</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H4">
+        <v>180</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="4">
         <v>38893</v>
       </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
       <c r="C5" t="s">
         <v>51</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>240</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="4">
         <v>39281</v>
       </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
       <c r="C6" t="s">
         <v>52</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>180</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="4">
         <v>39307</v>
       </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
       <c r="C7" t="s">
         <v>49</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="L7" t="s">
+      <c r="E7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="O7" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15">
       <c r="A8" s="4">
         <v>39307</v>
       </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
       <c r="C8" t="s">
         <v>48</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="L8" t="s">
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="O8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15">
       <c r="A9" s="4">
         <v>39307</v>
       </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
       <c r="C9" t="s">
         <v>51</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
       </c>
-      <c r="L9" t="s">
+      <c r="E9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="O9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15">
       <c r="A10" s="4">
         <v>39307</v>
       </c>
+      <c r="B10" t="s">
+        <v>83</v>
+      </c>
       <c r="C10" t="s">
         <v>54</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
-      <c r="L10" t="s">
+      <c r="E10" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="O10" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15">
+      <c r="A11" s="4">
+        <v>39307</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <v>180</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="4">
+        <v>36744</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12">
+        <v>6</v>
+      </c>
+      <c r="H12">
+        <v>480</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="4">
+        <v>36744</v>
+      </c>
+      <c r="B13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13">
+        <v>6</v>
+      </c>
+      <c r="H13">
+        <v>180</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="4">
+        <v>37829</v>
+      </c>
+      <c r="B14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>240</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="4">
+        <v>37889</v>
+      </c>
+      <c r="B15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" t="s">
+        <v>94</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H15">
+        <v>360</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="4">
+        <v>39219</v>
+      </c>
+      <c r="B16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <v>150</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="4">
+        <v>39281</v>
+      </c>
+      <c r="B17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" t="s">
+        <v>99</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H17">
+        <v>180</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="4"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" s="4"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="4"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="4"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="4"/>
-      <c r="B28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="4"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" s="4"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1">
       <c r="A33" s="4"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1">
       <c r="A34" s="4"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1">
       <c r="A35" s="4"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1">
       <c r="A36" s="4"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1">
       <c r="A37" s="4"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1">
       <c r="A38" s="4"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1">
       <c r="A39" s="4"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1">
       <c r="A40" s="4"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1">
       <c r="A41" s="4"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1">
       <c r="A42" s="4"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1">
       <c r="A43" s="4"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1">
       <c r="A44" s="4"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1">
       <c r="A45" s="4"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1">
       <c r="A46" s="4"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1">
       <c r="A47" s="4"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1">
       <c r="A48" s="4"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1">
       <c r="A49" s="4"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1">
       <c r="A50" s="4"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1">
       <c r="A51" s="4"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1">
       <c r="A52" s="4"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1">
       <c r="A53" s="4"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1">
       <c r="A54" s="4"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1">
       <c r="A55" s="4"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1">
       <c r="A56" s="4"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1">
       <c r="A57" s="4"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1">
       <c r="A58" s="4"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1">
       <c r="A59" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated reduction status list
Added some more info related to MC3PO reductions
</commit_message>
<xml_diff>
--- a/Reduction Notes/Reduction_Status_List.xlsx
+++ b/Reduction Notes/Reduction_Status_List.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26018"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dawson/Git/SuprimeCam/Reduction Notes/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26060" yWindow="8680" windowWidth="17420" windowHeight="16880" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="27600" yWindow="12300" windowWidth="16220" windowHeight="10660" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Radio Relic Sample" sheetId="1" r:id="rId1"/>
     <sheet name="MC3PO Sample" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="107">
   <si>
     <t>Semester</t>
   </si>
@@ -172,24 +177,15 @@
     <t>W-C-IC</t>
   </si>
   <si>
-    <t>check other F4</t>
-  </si>
-  <si>
     <t>W-J-V</t>
   </si>
   <si>
     <t>W-S-Z+</t>
   </si>
   <si>
-    <t>short</t>
-  </si>
-  <si>
     <t>W-J-B</t>
   </si>
   <si>
-    <t>mixed length exposures</t>
-  </si>
-  <si>
     <t>FRAMEID_start</t>
   </si>
   <si>
@@ -338,6 +334,18 @@
   </si>
   <si>
     <t>Total Exp (m)</t>
+  </si>
+  <si>
+    <t>There is no JVO reduction prior to 2001.</t>
+  </si>
+  <si>
+    <t>Flat Raw</t>
+  </si>
+  <si>
+    <t>Flat Reduced</t>
+  </si>
+  <si>
+    <t>short, don't bother</t>
   </si>
 </sst>
 </file>
@@ -718,7 +726,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -732,7 +740,7 @@
       <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
@@ -744,7 +752,7 @@
     <col min="10" max="10" width="75.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -776,7 +784,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -800,7 +808,7 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -824,7 +832,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -848,7 +856,7 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -870,7 +878,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -890,7 +898,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -910,7 +918,7 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -934,7 +942,7 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -960,7 +968,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -984,7 +992,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1008,7 +1016,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1032,7 +1040,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -1056,7 +1064,7 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -1080,7 +1088,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1104,7 +1112,7 @@
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1124,7 +1132,7 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>39513</v>
       </c>
@@ -1144,7 +1152,7 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>40279</v>
       </c>
@@ -1164,7 +1172,7 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>40637</v>
       </c>
@@ -1184,7 +1192,7 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -1208,7 +1216,7 @@
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -1232,7 +1240,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -1256,7 +1264,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
@@ -1282,7 +1290,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -1304,7 +1312,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -1324,7 +1332,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>8</v>
       </c>
@@ -1348,7 +1356,7 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -1372,7 +1380,7 @@
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -1394,7 +1402,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -1414,7 +1422,7 @@
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -1438,7 +1446,7 @@
       <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -1462,7 +1470,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -1486,7 +1494,7 @@
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -1506,7 +1514,7 @@
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
@@ -1526,7 +1534,7 @@
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -1546,7 +1554,7 @@
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -1566,7 +1574,7 @@
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -1588,7 +1596,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>34</v>
       </c>
@@ -1608,7 +1616,7 @@
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>34</v>
       </c>
@@ -1628,7 +1636,7 @@
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>34</v>
       </c>
@@ -1648,7 +1656,7 @@
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>34</v>
       </c>
@@ -1670,7 +1678,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>34</v>
       </c>
@@ -1690,7 +1698,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>34</v>
       </c>
@@ -1712,7 +1720,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>34</v>
       </c>
@@ -1732,7 +1740,7 @@
       <c r="I44" s="2"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>34</v>
       </c>
@@ -1754,7 +1762,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>34</v>
       </c>
@@ -1774,7 +1782,7 @@
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
         <v>39</v>
@@ -1796,34 +1804,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O59"/>
+  <dimension ref="A1:P59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="13.6640625" customWidth="1"/>
     <col min="8" max="8" width="6.1640625" customWidth="1"/>
     <col min="9" max="9" width="12.83203125" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
-    <col min="12" max="12" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="16">
+    <row r="1" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1837,40 +1840,43 @@
         <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>38476</v>
       </c>
@@ -1884,10 +1890,10 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G2">
         <f>(RIGHT(F2,LEN(F2)-4)-RIGHT(E2,LEN(E2)-4)+1)/10</f>
@@ -1901,10 +1907,13 @@
         <v>9</v>
       </c>
       <c r="J2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>37829</v>
       </c>
@@ -1918,10 +1927,10 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G17" si="0">(RIGHT(F3,LEN(F3)-4)-RIGHT(E3,LEN(E3)-4)+1)/10</f>
@@ -1934,13 +1943,19 @@
         <f t="shared" ref="I3:I17" si="1">G3*H3/60</f>
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>38187</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
         <v>49</v>
@@ -1949,10 +1964,10 @@
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -1965,25 +1980,31 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="J4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>38893</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
@@ -1996,25 +2017,31 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="J5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>39281</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
@@ -2027,13 +2054,19 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="J6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>39307</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
         <v>49</v>
@@ -2042,10 +2075,10 @@
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -2058,16 +2091,16 @@
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="O7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="P7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>39307</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
         <v>48</v>
@@ -2076,10 +2109,10 @@
         <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
@@ -2092,28 +2125,28 @@
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="O8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="P8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>39307</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
@@ -2126,28 +2159,28 @@
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="O9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="P9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>39307</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
@@ -2160,28 +2193,28 @@
         <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
-      <c r="O10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="P10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>39307</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
@@ -2194,8 +2227,11 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="J11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>36744</v>
       </c>
@@ -2209,10 +2245,10 @@
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F12" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G12">
         <v>6</v>
@@ -2224,13 +2260,19 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="J12" t="s">
+        <v>12</v>
+      </c>
+      <c r="P12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>36744</v>
       </c>
       <c r="B13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C13" t="s">
         <v>49</v>
@@ -2239,10 +2281,10 @@
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G13">
         <v>6</v>
@@ -2254,25 +2296,31 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="J13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>37829</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
@@ -2285,25 +2333,31 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="J14" t="s">
+        <v>12</v>
+      </c>
+      <c r="K14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>37889</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
@@ -2316,13 +2370,19 @@
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="J15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>39219</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C16" t="s">
         <v>48</v>
@@ -2331,10 +2391,10 @@
         <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F16" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
@@ -2347,25 +2407,31 @@
         <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>39281</v>
       </c>
       <c r="B17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
@@ -2378,140 +2444,141 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17" t="s">
+        <v>12</v>
+      </c>
+      <c r="K17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="4"/>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="4"/>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="4"/>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" s="4"/>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished a2355 archival reduction
</commit_message>
<xml_diff>
--- a/Reduction Notes/Reduction_Status_List.xlsx
+++ b/Reduction Notes/Reduction_Status_List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="27600" yWindow="12300" windowWidth="16220" windowHeight="10660" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="16360" yWindow="4480" windowWidth="16220" windowHeight="10660" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Radio Relic Sample" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="109">
   <si>
     <t>Semester</t>
   </si>
@@ -346,6 +346,12 @@
   </si>
   <si>
     <t>short, don't bother</t>
+  </si>
+  <si>
+    <t>Downloaded FL1-4 some frames were rejected as part of the JVO reduction.</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -355,7 +361,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mmm\-dd;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -390,6 +396,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -408,7 +421,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -430,15 +443,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -449,6 +465,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -459,6 +476,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -736,7 +754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
@@ -1811,13 +1829,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="13.6640625" customWidth="1"/>
     <col min="8" max="8" width="6.1640625" customWidth="1"/>
     <col min="9" max="9" width="12.83203125" customWidth="1"/>
@@ -1912,6 +1931,18 @@
       <c r="K2" t="s">
         <v>12</v>
       </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>108</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="4">

</xml_diff>

<commit_message>
finished macsj2243 and macsj2228 reductions
</commit_message>
<xml_diff>
--- a/Reduction Notes/Reduction_Status_List.xlsx
+++ b/Reduction Notes/Reduction_Status_List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26018"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40" yWindow="7540" windowWidth="25080" windowHeight="13620" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="880" yWindow="14200" windowWidth="25080" windowHeight="13620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Radio Relic Sample" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="111">
   <si>
     <t>Semester</t>
   </si>
@@ -355,6 +355,9 @@
   </si>
   <si>
     <t>I don't think that this is really necessary given the 48min exposure in 2000</t>
+  </si>
+  <si>
+    <t>I used this as the deepband during reduction since the 2000aug RC band only had 8 chips.</t>
   </si>
 </sst>
 </file>
@@ -1833,7 +1836,7 @@
   <dimension ref="A1:P59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2330,6 +2333,15 @@
       <c r="J12" t="s">
         <v>12</v>
       </c>
+      <c r="K12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" t="s">
+        <v>12</v>
+      </c>
       <c r="P12" t="s">
         <v>103</v>
       </c>
@@ -2366,6 +2378,15 @@
       <c r="J13" t="s">
         <v>12</v>
       </c>
+      <c r="K13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" t="s">
+        <v>12</v>
+      </c>
+      <c r="M13" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
@@ -2403,6 +2424,12 @@
       <c r="K14" t="s">
         <v>12</v>
       </c>
+      <c r="L14" t="s">
+        <v>12</v>
+      </c>
+      <c r="M14" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
@@ -2440,6 +2467,15 @@
       <c r="K15" t="s">
         <v>12</v>
       </c>
+      <c r="L15" t="s">
+        <v>12</v>
+      </c>
+      <c r="M15" t="s">
+        <v>12</v>
+      </c>
+      <c r="P15" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
@@ -2477,11 +2513,17 @@
       <c r="K16" t="s">
         <v>12</v>
       </c>
+      <c r="L16" t="s">
+        <v>12</v>
+      </c>
+      <c r="M16" t="s">
+        <v>12</v>
+      </c>
       <c r="P16" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>39281</v>
       </c>
@@ -2517,50 +2559,56 @@
       <c r="K17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17" t="s">
+        <v>12</v>
+      </c>
+      <c r="M17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
minor changes to RELICS reduction list
</commit_message>
<xml_diff>
--- a/Reduction Notes/Reduction_Status_List.xlsx
+++ b/Reduction Notes/Reduction_Status_List.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="680" windowWidth="20280" windowHeight="22020" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="420" yWindow="560" windowWidth="14720" windowHeight="19900" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Radio Relic Sample" sheetId="1" r:id="rId1"/>
@@ -5698,7 +5698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q125"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -10247,8 +10247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10270,7 +10270,7 @@
     <col min="15" max="15" width="0" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="13.33203125" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="11.6640625" customWidth="1"/>
-    <col min="18" max="18" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="76" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated Reduction Status List with new MC3PO reductions.
</commit_message>
<xml_diff>
--- a/Reduction Notes/Reduction_Status_List.xlsx
+++ b/Reduction Notes/Reduction_Status_List.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="420" yWindow="560" windowWidth="31600" windowHeight="19900" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="3160" windowWidth="22280" windowHeight="16320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Radio Relic Sample" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1856" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1888" uniqueCount="651">
   <si>
     <t>Semester</t>
   </si>
@@ -2183,8 +2183,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2327,7 +2331,7 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2344,6 +2348,8 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2360,6 +2366,8 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="23">
@@ -3076,7 +3084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="P48" sqref="P48"/>
     </sheetView>
   </sheetViews>
@@ -6243,8 +6251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q125"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView tabSelected="1" topLeftCell="B47" workbookViewId="0">
+      <selection activeCell="O71" sqref="O71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8767,10 +8775,18 @@
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
-      <c r="K64" s="24"/>
-      <c r="L64" s="24"/>
-      <c r="M64" s="24"/>
-      <c r="N64" s="24"/>
+      <c r="K64" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="L64" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="M64" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="N64" s="24" t="s">
+        <v>12</v>
+      </c>
       <c r="O64" s="24"/>
       <c r="P64" s="24"/>
       <c r="Q64" s="24" t="s">
@@ -8808,10 +8824,18 @@
         <f t="shared" si="7"/>
         <v>16</v>
       </c>
-      <c r="K65" s="24"/>
-      <c r="L65" s="24"/>
-      <c r="M65" s="24"/>
-      <c r="N65" s="24"/>
+      <c r="K65" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="L65" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="M65" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="N65" s="24" t="s">
+        <v>12</v>
+      </c>
       <c r="O65" s="24"/>
       <c r="P65" s="24"/>
       <c r="Q65" s="24" t="s">
@@ -8849,10 +8873,18 @@
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
-      <c r="K66" s="24"/>
-      <c r="L66" s="24"/>
-      <c r="M66" s="24"/>
-      <c r="N66" s="24"/>
+      <c r="K66" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="L66" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="M66" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="N66" s="24" t="s">
+        <v>12</v>
+      </c>
       <c r="O66" s="24"/>
       <c r="P66" s="24"/>
       <c r="Q66" s="24" t="s">
@@ -8972,10 +9004,18 @@
         <f t="shared" si="7"/>
         <v>28</v>
       </c>
-      <c r="K69" s="26"/>
-      <c r="L69" s="26"/>
-      <c r="M69" s="26"/>
-      <c r="N69" s="26"/>
+      <c r="K69" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="L69" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="M69" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="N69" s="26" t="s">
+        <v>12</v>
+      </c>
       <c r="O69" s="26"/>
       <c r="P69" s="26"/>
       <c r="Q69" s="26" t="s">
@@ -9013,10 +9053,18 @@
         <f t="shared" si="7"/>
         <v>28</v>
       </c>
-      <c r="K70" s="26"/>
-      <c r="L70" s="26"/>
-      <c r="M70" s="26"/>
-      <c r="N70" s="26"/>
+      <c r="K70" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="L70" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="M70" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="N70" s="26" t="s">
+        <v>12</v>
+      </c>
       <c r="O70" s="26"/>
       <c r="P70" s="26"/>
       <c r="Q70" s="26" t="s">
@@ -9054,10 +9102,18 @@
         <f t="shared" si="7"/>
         <v>36</v>
       </c>
-      <c r="K71" s="26"/>
-      <c r="L71" s="26"/>
-      <c r="M71" s="26"/>
-      <c r="N71" s="26"/>
+      <c r="K71" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="L71" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="M71" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="N71" s="26" t="s">
+        <v>12</v>
+      </c>
       <c r="O71" s="26"/>
       <c r="P71" s="26"/>
       <c r="Q71" s="26" t="s">
@@ -10066,10 +10122,18 @@
         <f t="shared" si="12"/>
         <v>48</v>
       </c>
-      <c r="K96" s="24"/>
-      <c r="L96" s="24"/>
-      <c r="M96" s="24"/>
-      <c r="N96" s="24"/>
+      <c r="K96" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="L96" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="M96" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="N96" s="24" t="s">
+        <v>12</v>
+      </c>
       <c r="O96" s="24"/>
       <c r="P96" s="24"/>
       <c r="Q96" s="24" t="s">
@@ -10107,10 +10171,18 @@
         <f t="shared" si="12"/>
         <v>36</v>
       </c>
-      <c r="K97" s="24"/>
-      <c r="L97" s="24"/>
-      <c r="M97" s="24"/>
-      <c r="N97" s="24"/>
+      <c r="K97" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="L97" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="M97" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="N97" s="24" t="s">
+        <v>12</v>
+      </c>
       <c r="O97" s="24"/>
       <c r="P97" s="24"/>
       <c r="Q97" s="24" t="s">
@@ -10792,8 +10864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15689,21 +15761,21 @@
         <f>'MC3PO Sample'!J69</f>
         <v>28</v>
       </c>
-      <c r="L101" s="14">
+      <c r="L101" s="14" t="str">
         <f>'MC3PO Sample'!K69</f>
-        <v>0</v>
-      </c>
-      <c r="M101" s="14">
+        <v>wd</v>
+      </c>
+      <c r="M101" s="14" t="str">
         <f>'MC3PO Sample'!L69</f>
-        <v>0</v>
-      </c>
-      <c r="N101" s="14">
+        <v>wd</v>
+      </c>
+      <c r="N101" s="14" t="str">
         <f>'MC3PO Sample'!M69</f>
-        <v>0</v>
-      </c>
-      <c r="O101" s="14">
+        <v>wd</v>
+      </c>
+      <c r="O101" s="14" t="str">
         <f>'MC3PO Sample'!N69</f>
-        <v>0</v>
+        <v>wd</v>
       </c>
       <c r="P101" s="14">
         <f>'MC3PO Sample'!O69</f>
@@ -15762,21 +15834,21 @@
         <f>'MC3PO Sample'!J70</f>
         <v>28</v>
       </c>
-      <c r="L102" s="14">
+      <c r="L102" s="14" t="str">
         <f>'MC3PO Sample'!K70</f>
-        <v>0</v>
-      </c>
-      <c r="M102" s="14">
+        <v>wd</v>
+      </c>
+      <c r="M102" s="14" t="str">
         <f>'MC3PO Sample'!L70</f>
-        <v>0</v>
-      </c>
-      <c r="N102" s="14">
+        <v>wd</v>
+      </c>
+      <c r="N102" s="14" t="str">
         <f>'MC3PO Sample'!M70</f>
-        <v>0</v>
-      </c>
-      <c r="O102" s="14">
+        <v>wd</v>
+      </c>
+      <c r="O102" s="14" t="str">
         <f>'MC3PO Sample'!N70</f>
-        <v>0</v>
+        <v>wd</v>
       </c>
       <c r="P102" s="14">
         <f>'MC3PO Sample'!O70</f>
@@ -15835,21 +15907,21 @@
         <f>'MC3PO Sample'!J71</f>
         <v>36</v>
       </c>
-      <c r="L103" s="14">
+      <c r="L103" s="14" t="str">
         <f>'MC3PO Sample'!K71</f>
-        <v>0</v>
-      </c>
-      <c r="M103" s="14">
+        <v>wd</v>
+      </c>
+      <c r="M103" s="14" t="str">
         <f>'MC3PO Sample'!L71</f>
-        <v>0</v>
-      </c>
-      <c r="N103" s="14">
+        <v>wd</v>
+      </c>
+      <c r="N103" s="14" t="str">
         <f>'MC3PO Sample'!M71</f>
-        <v>0</v>
-      </c>
-      <c r="O103" s="14">
+        <v>wd</v>
+      </c>
+      <c r="O103" s="14" t="str">
         <f>'MC3PO Sample'!N71</f>
-        <v>0</v>
+        <v>wd</v>
       </c>
       <c r="P103" s="14">
         <f>'MC3PO Sample'!O71</f>

</xml_diff>